<commit_message>
One student showed me his results.
</commit_message>
<xml_diff>
--- a/lab/lab1/lab01_Section1.xlsx
+++ b/lab/lab1/lab01_Section1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liumanni/Documents/CSE 220/cse220_2020fall/lab/lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF8D97D-83F0-8947-BE49-241960C34AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2101DD8-0205-6744-A78F-489DCEB7B2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{1C3543F5-1004-B644-A376-BBD6DC1ED258}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -543,7 +543,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,7 +553,7 @@
     <col min="4" max="4" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -575,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -586,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -630,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -652,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -663,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -707,18 +707,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>

</xml_diff>